<commit_message>
Convert phyla to dendrogram, cut tree at different heights
</commit_message>
<xml_diff>
--- a/data/sp2_cd_hit_cutoffs.xlsx
+++ b/data/sp2_cd_hit_cutoffs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robi0916/Documents/Wageningen_UR/github/check_a_dom_specificity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C1AF5ED-64A7-1F4F-82B6-544D43F801DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD77685-205B-4347-AC14-B0A22ED0A9A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14920"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="25440" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sp2_cd_hit_cutoffs" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1087,14 +1087,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BX11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>